<commit_message>
edit: change every code in Homepgae.py to UAT.py as it belongs originally on UAT Page, also change excel data to UAT only
</commit_message>
<xml_diff>
--- a/data/data_allregresion.xlsx
+++ b/data/data_allregresion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Collage Sucks\QA Testing\Streamlit-PorjectX_New\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180C7A38-5525-4F58-8467-B60BCCB3F152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBF77FB-298A-4CC3-80CF-58A28BF6D53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E23BE15B-BC97-48AF-9D6E-FC2B48AE82EB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>Tanggal</t>
   </si>
@@ -94,13 +94,16 @@
   </si>
   <si>
     <t>1/25/2025</t>
+  </si>
+  <si>
+    <t>1/31/2026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,8 +144,14 @@
       <color rgb="FF0070C0"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,8 +176,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -322,264 +337,73 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -896,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EAFB38C-7432-4904-B9FE-20B9788A0442}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A25"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,453 +735,501 @@
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="14">
         <v>0.2</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="29">
-        <v>0.1918</v>
-      </c>
-      <c r="E2" s="18">
-        <v>0.1691</v>
-      </c>
-      <c r="F2" s="19">
-        <v>1.78E-2</v>
+      <c r="D2" s="16">
+        <v>0.21240000000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.18729999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.95E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="30">
-        <v>0.1862</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0.17630000000000001</v>
-      </c>
-      <c r="F3" s="20">
-        <v>6.3E-3</v>
+      <c r="D3" s="17">
+        <v>0.1953</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.18709999999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6.1999999999999998E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="10">
         <v>0.4</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="21">
-        <v>0.41880000000000001</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.36520000000000002</v>
-      </c>
-      <c r="F4" s="20">
-        <v>4.7300000000000002E-2</v>
+      <c r="D4" s="1">
+        <v>0.47339999999999999</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.37990000000000002</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8.6599999999999996E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="13" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="21">
-        <v>0.40060000000000001</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0.3629</v>
-      </c>
-      <c r="F5" s="20">
-        <v>3.2800000000000003E-2</v>
+      <c r="D5" s="1">
+        <v>0.39460000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.32679999999999998</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6.08E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="10">
         <v>0.5</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="21">
-        <v>0.63729999999999998</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.54390000000000005</v>
-      </c>
-      <c r="F6" s="20">
-        <v>6.3200000000000006E-2</v>
+      <c r="D6" s="1">
+        <v>0.67610000000000003</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.51390000000000002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>8.8800000000000004E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="21">
-        <v>0.61229999999999996</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0.52470000000000006</v>
-      </c>
-      <c r="F7" s="20">
-        <v>5.8799999999999998E-2</v>
+      <c r="D7" s="1">
+        <v>0.63149999999999995</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="F7" s="1">
+        <v>9.2200000000000004E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="10">
         <v>0.6</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="21">
-        <v>0.75439999999999996</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.67630000000000001</v>
-      </c>
-      <c r="F8" s="20">
-        <v>6.7100000000000007E-2</v>
+      <c r="D8" s="2">
+        <v>0.68840000000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="16" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="22">
-        <v>0.77490000000000003</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0.68269999999999997</v>
-      </c>
-      <c r="F9" s="23">
-        <v>8.3500000000000005E-2</v>
+      <c r="D9" s="1">
+        <v>0.68840000000000001</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.55589999999999995</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.1212</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="10">
         <v>0.7</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="21">
-        <v>0.89549999999999996</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0.77569999999999995</v>
-      </c>
-      <c r="F10" s="20">
-        <v>8.8200000000000001E-2</v>
+      <c r="D10" s="18">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.66469999999999996</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0.115</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="13" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="21">
-        <v>0.86760000000000004</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0.76680000000000004</v>
-      </c>
-      <c r="F11" s="20">
-        <v>0.1011</v>
+      <c r="D11" s="19">
+        <v>0.73519999999999996</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0.57169999999999999</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0.1522</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="10">
         <v>0.8</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="21">
-        <v>0.91220000000000001</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0.84219999999999995</v>
-      </c>
-      <c r="F12" s="20">
-        <v>6.1800000000000001E-2</v>
+      <c r="D12" s="1">
+        <v>0.83689999999999998</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.751</v>
+      </c>
+      <c r="F12" s="1">
+        <v>7.6799999999999993E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="13" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="21">
-        <v>0.90429999999999999</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0.83189999999999997</v>
-      </c>
-      <c r="F13" s="20">
-        <v>6.3299999999999995E-2</v>
+      <c r="D13" s="1">
+        <v>0.81079999999999997</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.72089999999999999</v>
+      </c>
+      <c r="F13" s="1">
+        <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="10">
         <v>0.84</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="21">
-        <v>0.97340000000000004</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0.88090000000000002</v>
-      </c>
-      <c r="F14" s="20">
-        <v>6.2100000000000002E-2</v>
+      <c r="D14" s="1">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.79190000000000005</v>
+      </c>
+      <c r="F14" s="1">
+        <v>7.7200000000000005E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="13" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="21">
-        <v>0.96830000000000005</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0.87390000000000001</v>
-      </c>
-      <c r="F15" s="20">
-        <v>6.0199999999999997E-2</v>
+      <c r="D15" s="1">
+        <v>0.93189999999999995</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.77839999999999998</v>
+      </c>
+      <c r="F15" s="2">
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="10">
         <v>0.88</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="21">
-        <v>0.99029999999999996</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0.91020000000000001</v>
-      </c>
-      <c r="F16" s="20">
-        <v>5.0299999999999997E-2</v>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="20">
+        <v>0.83989999999999998</v>
+      </c>
+      <c r="F16" s="21">
+        <v>6.6900000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="13" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="21">
-        <v>0.98939999999999995</v>
-      </c>
-      <c r="E17" s="6">
-        <v>0.91720000000000002</v>
-      </c>
-      <c r="F17" s="20">
-        <v>4.1599999999999998E-2</v>
+      <c r="D17" s="1">
+        <v>0.99850000000000005</v>
+      </c>
+      <c r="E17" s="20">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="F17" s="21">
+        <v>5.74E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="10">
         <v>0.92</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="21">
-        <v>0.99860000000000004</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0.91990000000000005</v>
-      </c>
-      <c r="F18" s="20">
-        <v>4.58E-2</v>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.85329999999999995</v>
+      </c>
+      <c r="F18" s="19">
+        <v>6.1899999999999997E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="13" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="21">
-        <v>0.99650000000000005</v>
-      </c>
-      <c r="E19" s="6">
-        <v>0.91920000000000002</v>
-      </c>
-      <c r="F19" s="20">
-        <v>4.19E-2</v>
+      <c r="D19" s="1">
+        <v>0.99850000000000005</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.84819999999999995</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="10">
         <v>0.96</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="21">
-        <v>0.999</v>
-      </c>
-      <c r="E20" s="6">
-        <v>0.94</v>
-      </c>
-      <c r="F20" s="20">
-        <v>3.6900000000000002E-2</v>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.90310000000000001</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3.73E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="13" t="s">
+      <c r="A21" s="13"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6">
-        <v>0.94520000000000004</v>
-      </c>
-      <c r="F21" s="20">
-        <v>3.2800000000000003E-2</v>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2.69E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="12" t="s">
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="21">
-        <v>1</v>
-      </c>
-      <c r="E22" s="6">
-        <v>0.96509999999999996</v>
-      </c>
-      <c r="F22" s="20">
-        <v>2.7799999999999998E-2</v>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.97540000000000004</v>
+      </c>
+      <c r="F22" s="1">
+        <v>9.9000000000000008E-3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="13" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="22">
-        <v>1</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0.96660000000000001</v>
-      </c>
-      <c r="F23" s="23">
-        <v>2.7E-2</v>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.97740000000000005</v>
+      </c>
+      <c r="F23" s="1">
+        <v>9.4000000000000004E-3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="12" t="s">
+      <c r="B24" s="10">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="25"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="13" t="s">
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.98919999999999997</v>
+      </c>
+      <c r="F24" s="1">
+        <v>7.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="28"/>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.98970000000000002</v>
+      </c>
+      <c r="F25" s="1">
+        <v>7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="10">
+        <v>2</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
+  <mergeCells count="26">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
@@ -1374,10 +1246,13 @@
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>